<commit_message>
index bug fix in _calculate_bus_results_llg from results.py; corrected tests and updated some excel_files
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_1_four_bus_radial_grid_pf_sc_results_0_bus.xlsx
+++ b/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_1_four_bus_radial_grid_pf_sc_results_0_bus.xlsx
@@ -8670,37 +8670,37 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2.500000141879108</v>
+        <v>2.50000014187911</v>
       </c>
       <c r="D2">
-        <v>2.500000141879108</v>
+        <v>2.50000014187911</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>28.86751509776012</v>
+        <v>28.86751509776013</v>
       </c>
       <c r="G2">
-        <v>28.86751509776012</v>
+        <v>28.86751509776013</v>
       </c>
       <c r="H2">
-        <v>0.4428835862221404</v>
+        <v>0.4428835862221396</v>
       </c>
       <c r="I2">
-        <v>4.40271973851942</v>
+        <v>4.402719738519417</v>
       </c>
       <c r="J2">
-        <v>0.4378163569293868</v>
+        <v>0.4378163569293836</v>
       </c>
       <c r="K2">
-        <v>4.378163482534344</v>
+        <v>4.378163482534338</v>
       </c>
       <c r="L2">
-        <v>0.4378163569022844</v>
+        <v>0.4378163569022834</v>
       </c>
       <c r="M2">
-        <v>4.378163482487168</v>
+        <v>4.37816348248716</v>
       </c>
       <c r="N2">
         <v>0.9526279648091452</v>
@@ -8709,16 +8709,16 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.9526279648092945</v>
+        <v>0.9526279648092943</v>
       </c>
       <c r="Q2">
-        <v>-6.289991047015337E-13</v>
+        <v>-6.178256608332543E-13</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>179.9999999999919</v>
+        <v>179.999999999992</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -8771,7 +8771,7 @@
         <v>0.9526279648360654</v>
       </c>
       <c r="Q3">
-        <v>1.418502498641192E-09</v>
+        <v>1.418515578347718E-09</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -8821,16 +8821,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.9526279647734501</v>
+        <v>0.9526279647734502</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.9526279648449894</v>
+        <v>0.9526279648449892</v>
       </c>
       <c r="Q4">
-        <v>1.891543680729566E-09</v>
+        <v>1.891558592326962E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -8886,10 +8886,10 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.9526279648449894</v>
+        <v>0.9526279648449892</v>
       </c>
       <c r="Q5">
-        <v>1.891536204170228E-09</v>
+        <v>1.891553125357166E-09</v>
       </c>
       <c r="R5">
         <v>0</v>

</xml_diff>